<commit_message>
Data change lat - long
</commit_message>
<xml_diff>
--- a/public/stations.xlsx
+++ b/public/stations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nandalalsivadas/Desktop/fuel-map-app/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{04159734-999A-EB48-B783-B6BBEA04C5DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{91B2BFEE-049B-E74E-BB54-1A1A838626E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{9B18C86B-D065-B647-9723-E654086DE872}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16140" xr2:uid="{9B18C86B-D065-B647-9723-E654086DE872}"/>
   </bookViews>
   <sheets>
     <sheet name="stations" sheetId="1" r:id="rId1"/>
@@ -1708,8 +1708,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A922ACBE-E6A4-AA40-AF75-BFC5BA62349F}">
   <dimension ref="A1:K182"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="H41" sqref="H41"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="I41" sqref="I41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3123,10 +3123,10 @@
         <v>67</v>
       </c>
       <c r="F41">
-        <v>10.9434605</v>
+        <v>10.9882831</v>
       </c>
       <c r="G41">
-        <v>75.938909499999994</v>
+        <v>75.906533199999998</v>
       </c>
       <c r="H41">
         <v>88</v>

</xml_diff>

<commit_message>
Update stations.csv with latest sales data
</commit_message>
<xml_diff>
--- a/public/stations.xlsx
+++ b/public/stations.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nandalalsivadas/Desktop/fuel-map-app/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{B7C8F46E-A908-944A-930C-F5F2752B76BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{90D209EA-C578-4145-A726-5E6826426D1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4640" yWindow="500" windowWidth="28800" windowHeight="16140" xr2:uid="{9B18C86B-D065-B647-9723-E654086DE872}"/>
+    <workbookView xWindow="4680" yWindow="500" windowWidth="28800" windowHeight="16140" xr2:uid="{9B18C86B-D065-B647-9723-E654086DE872}"/>
   </bookViews>
   <sheets>
     <sheet name="stations" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">stations!$A$1:$K$906</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -1721,8 +1724,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A922ACBE-E6A4-AA40-AF75-BFC5BA62349F}">
   <dimension ref="A1:K906"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A786" workbookViewId="0">
-      <selection activeCell="G803" sqref="G803"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4454,10 +4457,10 @@
         <v>67</v>
       </c>
       <c r="F79">
-        <v>10.850793299999999</v>
+        <v>10.8866792</v>
       </c>
       <c r="G79">
-        <v>75.941027099999999</v>
+        <v>75.930557399999998</v>
       </c>
       <c r="H79">
         <v>50</v>
@@ -4558,6 +4561,12 @@
       <c r="E82" t="s">
         <v>67</v>
       </c>
+      <c r="F82">
+        <v>11.076765099999999</v>
+      </c>
+      <c r="G82">
+        <v>75.902970600000003</v>
+      </c>
       <c r="H82">
         <v>0</v>
       </c>
@@ -4727,6 +4736,12 @@
       <c r="E87" t="s">
         <v>152</v>
       </c>
+      <c r="F87">
+        <v>11.109537899999999</v>
+      </c>
+      <c r="G87">
+        <v>75.836205399999997</v>
+      </c>
       <c r="H87">
         <v>0</v>
       </c>
@@ -7188,6 +7203,12 @@
       <c r="E158" t="s">
         <v>239</v>
       </c>
+      <c r="F158">
+        <v>10.929333400000001</v>
+      </c>
+      <c r="G158">
+        <v>75.998249999999999</v>
+      </c>
       <c r="H158">
         <v>85</v>
       </c>
@@ -7514,6 +7535,12 @@
       <c r="E168" t="s">
         <v>246</v>
       </c>
+      <c r="F168">
+        <v>11.167624099999999</v>
+      </c>
+      <c r="G168">
+        <v>75.930183900000003</v>
+      </c>
       <c r="H168">
         <v>65</v>
       </c>
@@ -7706,6 +7733,12 @@
       <c r="E174" t="s">
         <v>246</v>
       </c>
+      <c r="F174">
+        <v>11.102840499999999</v>
+      </c>
+      <c r="G174">
+        <v>75.893086999999994</v>
+      </c>
       <c r="H174">
         <v>58</v>
       </c>
@@ -10681,10 +10714,10 @@
         <v>67</v>
       </c>
       <c r="F260">
-        <v>10.850793299999999</v>
+        <v>10.8866792</v>
       </c>
       <c r="G260">
-        <v>75.941027099999999</v>
+        <v>75.930557399999998</v>
       </c>
       <c r="H260">
         <v>0</v>
@@ -10785,6 +10818,12 @@
       <c r="E263" t="s">
         <v>67</v>
       </c>
+      <c r="F263">
+        <v>11.076765099999999</v>
+      </c>
+      <c r="G263">
+        <v>75.902970600000003</v>
+      </c>
       <c r="H263">
         <v>4</v>
       </c>
@@ -13415,6 +13454,12 @@
       <c r="E339" t="s">
         <v>239</v>
       </c>
+      <c r="F339">
+        <v>10.929334000000001</v>
+      </c>
+      <c r="G339">
+        <v>75.998249999999999</v>
+      </c>
       <c r="H339">
         <v>80</v>
       </c>
@@ -13741,6 +13786,12 @@
       <c r="E349" t="s">
         <v>246</v>
       </c>
+      <c r="F349">
+        <v>11.167624099999999</v>
+      </c>
+      <c r="G349">
+        <v>75.930183900000003</v>
+      </c>
       <c r="H349">
         <v>65</v>
       </c>
@@ -13933,6 +13984,12 @@
       <c r="E355" t="s">
         <v>246</v>
       </c>
+      <c r="F355">
+        <v>11.102840499999999</v>
+      </c>
+      <c r="G355">
+        <v>75.893086999999994</v>
+      </c>
       <c r="H355">
         <v>58</v>
       </c>
@@ -16908,10 +16965,10 @@
         <v>67</v>
       </c>
       <c r="F441">
-        <v>10.850793299999999</v>
+        <v>10.8866792</v>
       </c>
       <c r="G441">
-        <v>75.941027099999999</v>
+        <v>75.930557399999998</v>
       </c>
       <c r="H441">
         <v>4</v>
@@ -17012,6 +17069,12 @@
       <c r="E444" t="s">
         <v>67</v>
       </c>
+      <c r="F444">
+        <v>11.076765099999999</v>
+      </c>
+      <c r="G444">
+        <v>75.902970600000003</v>
+      </c>
       <c r="H444">
         <v>0</v>
       </c>
@@ -17181,6 +17244,12 @@
       <c r="E449" t="s">
         <v>152</v>
       </c>
+      <c r="F449">
+        <v>11.109537899999999</v>
+      </c>
+      <c r="G449">
+        <v>75.836205399999997</v>
+      </c>
       <c r="H449">
         <v>0</v>
       </c>
@@ -19473,6 +19542,12 @@
       <c r="E515" t="s">
         <v>152</v>
       </c>
+      <c r="F515">
+        <v>10.9898428</v>
+      </c>
+      <c r="G515">
+        <v>76.021480299999993</v>
+      </c>
       <c r="H515">
         <v>0</v>
       </c>
@@ -19642,6 +19717,12 @@
       <c r="E520" t="s">
         <v>239</v>
       </c>
+      <c r="F520">
+        <v>10.929334000000001</v>
+      </c>
+      <c r="G520">
+        <v>75.998249999999999</v>
+      </c>
       <c r="H520">
         <v>80</v>
       </c>
@@ -19968,6 +20049,12 @@
       <c r="E530" t="s">
         <v>246</v>
       </c>
+      <c r="F530">
+        <v>11.167624099999999</v>
+      </c>
+      <c r="G530">
+        <v>75.930183900000003</v>
+      </c>
       <c r="H530">
         <v>75</v>
       </c>
@@ -20160,6 +20247,12 @@
       <c r="E536" t="s">
         <v>246</v>
       </c>
+      <c r="F536">
+        <v>11.102840499999999</v>
+      </c>
+      <c r="G536">
+        <v>75.893086999999994</v>
+      </c>
       <c r="H536">
         <v>60</v>
       </c>
@@ -23134,6 +23227,12 @@
       <c r="E622" t="s">
         <v>67</v>
       </c>
+      <c r="F622">
+        <v>10.8866792</v>
+      </c>
+      <c r="G622">
+        <v>75.930557399999998</v>
+      </c>
       <c r="H622">
         <v>0</v>
       </c>
@@ -23233,6 +23332,12 @@
       <c r="E625" t="s">
         <v>67</v>
       </c>
+      <c r="F625">
+        <v>11.076765099999999</v>
+      </c>
+      <c r="G625">
+        <v>75.902970600000003</v>
+      </c>
       <c r="H625">
         <v>0</v>
       </c>
@@ -25863,6 +25968,12 @@
       <c r="E701" t="s">
         <v>239</v>
       </c>
+      <c r="F701">
+        <v>10.929334000000001</v>
+      </c>
+      <c r="G701">
+        <v>75.998249999999999</v>
+      </c>
       <c r="H701">
         <v>80</v>
       </c>
@@ -26189,6 +26300,12 @@
       <c r="E711" t="s">
         <v>246</v>
       </c>
+      <c r="F711">
+        <v>11.167624099999999</v>
+      </c>
+      <c r="G711">
+        <v>75.930183900000003</v>
+      </c>
       <c r="H711">
         <v>85</v>
       </c>
@@ -26381,6 +26498,12 @@
       <c r="E717" t="s">
         <v>246</v>
       </c>
+      <c r="F717">
+        <v>11.1028425</v>
+      </c>
+      <c r="G717">
+        <v>75.893092300000006</v>
+      </c>
       <c r="H717">
         <v>65</v>
       </c>
@@ -29460,6 +29583,12 @@
       <c r="E806" t="s">
         <v>67</v>
       </c>
+      <c r="F806">
+        <v>11.076765099999999</v>
+      </c>
+      <c r="G806">
+        <v>75.902970600000003</v>
+      </c>
       <c r="H806">
         <v>0</v>
       </c>
@@ -29629,6 +29758,12 @@
       <c r="E811" t="s">
         <v>152</v>
       </c>
+      <c r="F811">
+        <v>11.1076353</v>
+      </c>
+      <c r="G811">
+        <v>75.837608799999998</v>
+      </c>
       <c r="H811">
         <v>0</v>
       </c>
@@ -31921,6 +32056,12 @@
       <c r="E877" t="s">
         <v>152</v>
       </c>
+      <c r="F877">
+        <v>10.9897204</v>
+      </c>
+      <c r="G877">
+        <v>76.021091400000003</v>
+      </c>
       <c r="H877">
         <v>0</v>
       </c>
@@ -32090,6 +32231,12 @@
       <c r="E882" t="s">
         <v>239</v>
       </c>
+      <c r="F882">
+        <v>10.929334000000001</v>
+      </c>
+      <c r="G882">
+        <v>75.998249999999999</v>
+      </c>
       <c r="H882">
         <v>90</v>
       </c>
@@ -32416,6 +32563,12 @@
       <c r="E892" t="s">
         <v>246</v>
       </c>
+      <c r="F892">
+        <v>11.167624099999999</v>
+      </c>
+      <c r="G892">
+        <v>75.930183900000003</v>
+      </c>
       <c r="H892">
         <v>80</v>
       </c>
@@ -32509,6 +32662,12 @@
       <c r="E895" t="s">
         <v>246</v>
       </c>
+      <c r="F895">
+        <v>11.1295825</v>
+      </c>
+      <c r="G895">
+        <v>76.004713499999994</v>
+      </c>
       <c r="H895">
         <v>115</v>
       </c>
@@ -32607,6 +32766,12 @@
       </c>
       <c r="E898" t="s">
         <v>246</v>
+      </c>
+      <c r="F898">
+        <v>11.102840499999999</v>
+      </c>
+      <c r="G898">
+        <v>75.893086999999994</v>
       </c>
       <c r="H898">
         <v>64</v>

</xml_diff>